<commit_message>
Adding Appendix C HumMod data and the relevant changed DES files
</commit_message>
<xml_diff>
--- a/appendices/C_exercise_tolerance/C_exercise_tolerance_data.xlsx
+++ b/appendices/C_exercise_tolerance/C_exercise_tolerance_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
   <si>
     <t>Balke and Ware</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Muscle Flow(mL/min)</t>
   </si>
   <si>
-    <t>Temperature(C˚)</t>
-  </si>
-  <si>
     <t>124/79</t>
   </si>
   <si>
@@ -103,6 +100,36 @@
   </si>
   <si>
     <t>162/96</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>127/87</t>
+  </si>
+  <si>
+    <t>129/65</t>
+  </si>
+  <si>
+    <t>130/64</t>
+  </si>
+  <si>
+    <t>Temperature(F˚)</t>
+  </si>
+  <si>
+    <t>HumMod cannot bring the treadmill grade above 15%</t>
+  </si>
+  <si>
+    <t>133/66</t>
+  </si>
+  <si>
+    <t>I changed the treadmill DES file in display to allow a larger grade to be accomplished. However, in HumMod, any grade above 10% will not increase the workload of the patient</t>
+  </si>
+  <si>
+    <t>134/67</t>
   </si>
 </sst>
 </file>
@@ -124,12 +151,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -209,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -233,6 +266,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -529,23 +574,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
       <c r="H1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1">
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -582,8 +645,44 @@
       <c r="M2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="30.75" thickBot="1">
+      <c r="Q2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="30.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -620,8 +719,44 @@
       <c r="M3" s="4">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+      <c r="Q3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="T3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="U3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="V3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -658,8 +793,44 @@
       <c r="M4" s="5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="60.75" thickBot="1">
+      <c r="Q4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="60.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -682,22 +853,58 @@
         <v>15</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="75.75" thickBot="1">
+      <c r="Q5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="6">
+        <v>76</v>
+      </c>
+      <c r="S5" s="6">
+        <v>142</v>
+      </c>
+      <c r="T5" s="6">
+        <v>147</v>
+      </c>
+      <c r="U5" s="6">
+        <v>147</v>
+      </c>
+      <c r="V5" s="6">
+        <v>146</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC5" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="75.75" thickBot="1">
       <c r="H6" s="3" t="s">
         <v>16</v>
       </c>
@@ -716,8 +923,26 @@
       <c r="M6" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="45.75" thickBot="1">
+      <c r="X6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>5724</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>16905</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>18179</v>
+      </c>
+      <c r="AB6" s="6">
+        <v>18406</v>
+      </c>
+      <c r="AC6" s="6">
+        <v>18480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="45.75" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -742,8 +967,32 @@
       <c r="M7" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="60.75" thickBot="1">
+      <c r="Q7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="R7" s="12">
+        <v>0.15532407407407409</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y7" s="6">
+        <v>76</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>142</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>147</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>147</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="60.75" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -768,8 +1017,32 @@
       <c r="M8" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="75.75" thickBot="1">
+      <c r="Q8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="1">
+        <v>68888</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y8" s="6">
+        <v>76</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>119</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>123</v>
+      </c>
+      <c r="AB8" s="6">
+        <v>125</v>
+      </c>
+      <c r="AC8" s="6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="75.75" thickBot="1">
       <c r="H9" s="3" t="s">
         <v>19</v>
       </c>
@@ -788,8 +1061,26 @@
       <c r="M9" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="60.75" thickBot="1">
+      <c r="X9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>12.1</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>29.3</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>29.6</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="60.75" thickBot="1">
       <c r="H10" s="3" t="s">
         <v>20</v>
       </c>
@@ -808,8 +1099,26 @@
       <c r="M10" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="45.75" thickBot="1">
+      <c r="X10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>6.7</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>51.7</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>61.5</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="AC10" s="6">
+        <v>69.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="45.75" thickBot="1">
       <c r="H11" s="3" t="s">
         <v>21</v>
       </c>
@@ -828,8 +1137,26 @@
       <c r="M11" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="45.75" thickBot="1">
+      <c r="X11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>0.192</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>0.193</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>0.19</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="45.75" thickBot="1">
       <c r="H12" s="3" t="s">
         <v>22</v>
       </c>
@@ -848,8 +1175,26 @@
       <c r="M12" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="45.75" thickBot="1">
+      <c r="X12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y12" s="6">
+        <v>0.151</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>7.8E-2</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="AB12" s="6">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AC12" s="6">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="45.75" thickBot="1">
       <c r="H13" s="3" t="s">
         <v>23</v>
       </c>
@@ -868,10 +1213,28 @@
       <c r="M13" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="45.75" thickBot="1">
+      <c r="X13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>840</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>13537</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>14812</v>
+      </c>
+      <c r="AB13" s="6">
+        <v>14873</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>14862</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="45.75" thickBot="1">
       <c r="H14" s="3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="I14" s="6">
         <v>98.5</v>
@@ -888,8 +1251,66 @@
       <c r="M14" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="X14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y14" s="6">
+        <v>98.5</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>99</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="AB14" s="6">
+        <v>100</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>100.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="X16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+    </row>
+    <row r="18" spans="24:29">
+      <c r="X18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+    </row>
+    <row r="19" spans="24:29">
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+    </row>
+    <row r="20" spans="24:29">
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="X16:AC16"/>
+    <mergeCell ref="X18:AC20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding percentage data to Appendix C
</commit_message>
<xml_diff>
--- a/appendices/C_exercise_tolerance/C_exercise_tolerance_data.xlsx
+++ b/appendices/C_exercise_tolerance/C_exercise_tolerance_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
   <si>
     <t>Balke and Ware</t>
   </si>
@@ -130,13 +130,19 @@
   </si>
   <si>
     <t>134/67</t>
+  </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +155,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -239,10 +252,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -268,6 +282,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -277,14 +294,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -574,15 +621,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC20"/>
+  <dimension ref="A1:AL20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" thickBot="1">
+    <row r="1" spans="1:38" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,8 +654,14 @@
       <c r="AB1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" ht="15.75" thickBot="1">
+      <c r="AG1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -681,8 +734,26 @@
       <c r="AC2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" ht="30.75" thickBot="1">
+      <c r="AG2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="30.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -755,8 +826,26 @@
       <c r="AC3" s="4">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" thickBot="1">
+      <c r="AG3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="AJ3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="AK3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -829,8 +918,26 @@
       <c r="AC4" s="5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" ht="60.75" thickBot="1">
+      <c r="AG4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" ht="60.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -903,8 +1010,26 @@
       <c r="AC5" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" ht="75.75" thickBot="1">
+      <c r="AG5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" ht="75.75" thickBot="1">
       <c r="H6" s="3" t="s">
         <v>16</v>
       </c>
@@ -941,8 +1066,30 @@
       <c r="AC6" s="6">
         <v>18480</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" ht="45.75" thickBot="1">
+      <c r="AG6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH6" s="13">
+        <f>ABS((I6-Y6)/I6)</f>
+        <v>7.0707070707070704E-2</v>
+      </c>
+      <c r="AI6" s="13">
+        <f t="shared" ref="AI6:AI14" si="0">ABS((J6-Z6)/J6)</f>
+        <v>7.0004430660168371E-2</v>
+      </c>
+      <c r="AJ6" s="13">
+        <f t="shared" ref="AJ6:AJ14" si="1">ABS((K6-AA6)/K6)</f>
+        <v>7.2087816066845065E-3</v>
+      </c>
+      <c r="AK6" s="13">
+        <f t="shared" ref="AK6:AK14" si="2">ABS((L6-AB6)/L6)</f>
+        <v>0.14652694055457666</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="45.75" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -970,7 +1117,7 @@
       <c r="Q7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="9">
         <v>0.15532407407407409</v>
       </c>
       <c r="X7" s="3" t="s">
@@ -991,8 +1138,30 @@
       <c r="AC7" s="6">
         <v>146</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" ht="60.75" thickBot="1">
+      <c r="AG7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH7" s="13">
+        <f t="shared" ref="AH7:AH14" si="3">ABS((I7-Y7)/I7)</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="AI7" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4285714285714285E-2</v>
+      </c>
+      <c r="AJ7" s="13">
+        <f t="shared" si="1"/>
+        <v>8.1250000000000003E-2</v>
+      </c>
+      <c r="AK7" s="13">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="AL7" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="60.75" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1041,8 +1210,30 @@
       <c r="AC8" s="6">
         <v>126</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" ht="75.75" thickBot="1">
+      <c r="AG8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH8" s="13">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="AI8" s="13">
+        <f t="shared" si="0"/>
+        <v>5.3097345132743362E-2</v>
+      </c>
+      <c r="AJ8" s="13">
+        <f t="shared" si="1"/>
+        <v>6.9565217391304349E-2</v>
+      </c>
+      <c r="AK8" s="13">
+        <f t="shared" si="2"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="AL8" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="75.75" thickBot="1">
       <c r="H9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1079,8 +1270,30 @@
       <c r="AC9" s="6">
         <v>29.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" ht="60.75" thickBot="1">
+      <c r="AG9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH9" s="13">
+        <f t="shared" si="3"/>
+        <v>6.9230769230769262E-2</v>
+      </c>
+      <c r="AI9" s="13">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="AJ9" s="13">
+        <f t="shared" si="1"/>
+        <v>0.13823529411764704</v>
+      </c>
+      <c r="AK9" s="13">
+        <f t="shared" si="2"/>
+        <v>0.25999999999999995</v>
+      </c>
+      <c r="AL9" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" ht="60.75" thickBot="1">
       <c r="H10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1117,8 +1330,30 @@
       <c r="AC10" s="6">
         <v>69.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" ht="45.75" thickBot="1">
+      <c r="AG10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH10" s="13">
+        <f t="shared" si="3"/>
+        <v>3.0769230769230795E-2</v>
+      </c>
+      <c r="AI10" s="13">
+        <f t="shared" si="0"/>
+        <v>0.17147435897435892</v>
+      </c>
+      <c r="AJ10" s="13">
+        <f t="shared" si="1"/>
+        <v>0.28654292343387472</v>
+      </c>
+      <c r="AK10" s="13">
+        <f t="shared" si="2"/>
+        <v>0.45214521452145212</v>
+      </c>
+      <c r="AL10" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" ht="45.75" thickBot="1">
       <c r="H11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1155,8 +1390,30 @@
       <c r="AC11" s="6">
         <v>0.189</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" ht="45.75" thickBot="1">
+      <c r="AG11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH11" s="13">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="AI11" s="13">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="AJ11" s="13">
+        <f t="shared" si="1"/>
+        <v>8.0952380952380901E-2</v>
+      </c>
+      <c r="AK11" s="13">
+        <f t="shared" si="2"/>
+        <v>9.5238095238095191E-2</v>
+      </c>
+      <c r="AL11" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="45.75" thickBot="1">
       <c r="H12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1193,8 +1450,30 @@
       <c r="AC12" s="6">
         <v>6.4000000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" ht="45.75" thickBot="1">
+      <c r="AG12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH12" s="13">
+        <f t="shared" si="3"/>
+        <v>6.6666666666666732E-3</v>
+      </c>
+      <c r="AI12" s="13">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="AJ12" s="13">
+        <f t="shared" si="1"/>
+        <v>4.2857142857142892E-2</v>
+      </c>
+      <c r="AK12" s="13">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333412E-2</v>
+      </c>
+      <c r="AL12" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" ht="45.75" thickBot="1">
       <c r="H13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1231,8 +1510,30 @@
       <c r="AC13" s="6">
         <v>14862</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" ht="45.75" thickBot="1">
+      <c r="AG13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH13" s="13">
+        <f t="shared" si="3"/>
+        <v>0.34831460674157305</v>
+      </c>
+      <c r="AI13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.30451961067745975</v>
+      </c>
+      <c r="AJ13" s="13">
+        <f t="shared" si="1"/>
+        <v>0.23970539002343488</v>
+      </c>
+      <c r="AK13" s="13">
+        <f t="shared" si="2"/>
+        <v>9.2799412196914038E-2</v>
+      </c>
+      <c r="AL13" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="45.75" thickBot="1">
       <c r="H14" s="3" t="s">
         <v>33</v>
       </c>
@@ -1269,48 +1570,79 @@
       <c r="AC14" s="6">
         <v>100.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:29">
-      <c r="X16" s="9" t="s">
+      <c r="AG14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH14" s="13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="13">
+        <f t="shared" si="0"/>
+        <v>1.009081735620528E-3</v>
+      </c>
+      <c r="AJ14" s="13">
+        <f t="shared" si="1"/>
+        <v>4.0040040040040603E-3</v>
+      </c>
+      <c r="AK14" s="13">
+        <f t="shared" si="2"/>
+        <v>5.9642147117295657E-3</v>
+      </c>
+      <c r="AL14" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38">
+      <c r="X16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="10"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
     </row>
     <row r="18" spans="24:29">
-      <c r="X18" s="11" t="s">
+      <c r="X18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="11"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="12"/>
+      <c r="AC18" s="12"/>
     </row>
     <row r="19" spans="24:29">
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
-      <c r="AC19" s="11"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="12"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12"/>
     </row>
     <row r="20" spans="24:29">
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="11"/>
-      <c r="AB20" s="11"/>
-      <c r="AC20" s="11"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="X16:AC16"/>
     <mergeCell ref="X18:AC20"/>
   </mergeCells>
+  <conditionalFormatting sqref="AH6:AK14">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>